<commit_message>
cambios estructurales de Login.
</commit_message>
<xml_diff>
--- a/PRYHORASEXTRASV2/Recursos/Uploads/Plantilla_visitantes_frecuentes.xlsx
+++ b/PRYHORASEXTRASV2/Recursos/Uploads/Plantilla_visitantes_frecuentes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwin.martinez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1F9918-BBE5-4990-8FC6-CA97F7B5ED9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CC70A9-55BE-43D8-AD3A-5E8F5E011F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20490" yWindow="0" windowWidth="20520" windowHeight="10830" xr2:uid="{F6F24F53-FD26-47F4-882E-D1807F759693}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F6F24F53-FD26-47F4-882E-D1807F759693}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -62,26 +62,26 @@
     <t>FechaFin</t>
   </si>
   <si>
-    <t>probando visitante</t>
-  </si>
-  <si>
-    <t>frigorífico</t>
-  </si>
-  <si>
-    <t>visita zona arinas</t>
-  </si>
-  <si>
-    <t>factory s.a</t>
-  </si>
-  <si>
-    <t>zzz666</t>
+    <t xml:space="preserve">testeo </t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>FRIGORÍFICO</t>
+  </si>
+  <si>
+    <t>505050abc</t>
+  </si>
+  <si>
+    <t>testeo 5&amp;*/&amp;&amp; visitante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,14 +91,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,11 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +454,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,29 +496,26 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>78963214</v>
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="2">
-        <v>44905</v>
+        <v>44927</v>
       </c>
       <c r="I2" s="2">
-        <v>44936</v>
+        <v>44957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>